<commit_message>
fix the bug that prevented the users from signinup.
</commit_message>
<xml_diff>
--- a/xyz.xlsx
+++ b/xyz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Car Wash\Car Wash New JKI\Car Wash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D8782E-8EAB-4692-ABE1-AC7BC3269417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F4433A-0DBB-4ED9-9F94-E53337D0ADB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14460" yWindow="195" windowWidth="14340" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>sdgsdgv</t>
   </si>
   <si>
-    <t>fdsvfdsv</t>
-  </si>
-  <si>
-    <t>sdfsf</t>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>EFG</t>
+  </si>
+  <si>
+    <t>HIJ</t>
+  </si>
+  <si>
+    <t>QRS</t>
   </si>
 </sst>
 </file>
@@ -351,27 +357,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>